<commit_message>
Variant after new target names
</commit_message>
<xml_diff>
--- a/data/20151101_GEP00002/SLX-13774.haplotypeCaller.variants.xlsx
+++ b/data/20151101_GEP00002/SLX-13774.haplotypeCaller.variants.xlsx
@@ -308,7 +308,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>PTEN.off2</t>
+          <t>GRCh37.p13_chr9_88504079</t>
         </is>
       </c>
       <c r="AC2" t="n">
@@ -415,7 +415,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -3878,7 +3878,7 @@
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -4483,7 +4483,7 @@
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
@@ -4978,7 +4978,7 @@
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
@@ -5458,7 +5458,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U40" t="inlineStr">
@@ -5583,7 +5583,7 @@
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>PTEN.in</t>
+          <t>GRCh37.p13_chr10_89653730</t>
         </is>
       </c>
       <c r="U41" t="inlineStr">

</xml_diff>